<commit_message>
fixed a couple of things & updated scheduling s/s
</commit_message>
<xml_diff>
--- a/SSPHP Documentation/20241203_DCAP_Scheduling.xlsx
+++ b/SSPHP Documentation/20241203_DCAP_Scheduling.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelpritchard/Code/service-security-posture-hardening/SSPHP Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianpearl/GITHUB/service-security-posture-hardening/SSPHP Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3C6DEBC-F842-A546-9819-7A652329B52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A33BA4-02D7-E04B-AA9A-CFD41D8AE14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40960" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{E019FE81-96E6-EA40-88B3-D10E9033B9A2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="5" xr2:uid="{E019FE81-96E6-EA40-88B3-D10E9033B9A2}"/>
   </bookViews>
   <sheets>
     <sheet name="OVERALL" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="198">
   <si>
     <t>Starts</t>
   </si>
@@ -647,6 +647,9 @@
   </si>
   <si>
     <t>15 3 * * *</t>
+  </si>
+  <si>
+    <t>ssphp_create_bdmc_csv_DEV</t>
   </si>
 </sst>
 </file>
@@ -839,12 +842,12 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="5" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="9" fillId="7" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="9" fillId="7" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -863,10 +866,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1189,7 +1188,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E11" sqref="E11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1211,10 +1210,10 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="s">
         <v>13</v>
@@ -1494,7 +1493,7 @@
       <c r="A2" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>0.29166666666666669</v>
       </c>
       <c r="C2" t="s">
@@ -1507,7 +1506,7 @@
       <c r="A3" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>0.29166666666666669</v>
       </c>
       <c r="C3" t="s">
@@ -1705,7 +1704,7 @@
       <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>0.13541666666666666</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -1715,7 +1714,7 @@
       <c r="E2" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="23">
         <v>0.14583333333333334</v>
       </c>
       <c r="G2" s="10" t="s">
@@ -1725,7 +1724,7 @@
       <c r="I2" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="23">
         <v>0.14930555555555555</v>
       </c>
       <c r="K2" t="s">
@@ -1736,7 +1735,7 @@
       <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>0.13541666666666666</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -1746,7 +1745,7 @@
       <c r="E3" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="23">
         <v>0.14583333333333334</v>
       </c>
       <c r="G3" s="10" t="s">
@@ -1756,7 +1755,7 @@
       <c r="I3" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="23">
         <v>0.14930555555555555</v>
       </c>
       <c r="K3" t="s">
@@ -1767,7 +1766,7 @@
       <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>0.13541666666666666</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -1777,7 +1776,7 @@
       <c r="E4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>0.14583333333333334</v>
       </c>
       <c r="G4" s="10" t="s">
@@ -1787,7 +1786,7 @@
       <c r="I4" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="23">
         <v>0.14930555555555555</v>
       </c>
       <c r="K4" t="s">
@@ -1798,7 +1797,7 @@
       <c r="A5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>0.13541666666666666</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -1808,7 +1807,7 @@
       <c r="E5" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>0.14583333333333334</v>
       </c>
       <c r="G5" s="10" t="s">
@@ -1818,7 +1817,7 @@
       <c r="I5" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="23">
         <v>0.14930555555555555</v>
       </c>
       <c r="K5" t="s">
@@ -1829,7 +1828,7 @@
       <c r="A6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>0.13541666666666666</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -1841,7 +1840,7 @@
       <c r="I6" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="23">
         <v>0.14930555555555555</v>
       </c>
       <c r="K6" t="s">
@@ -1852,7 +1851,7 @@
       <c r="A7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>0.13541666666666666</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -1864,7 +1863,7 @@
       <c r="I7" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="23">
         <v>0.14930555555555555</v>
       </c>
       <c r="K7" t="s">
@@ -1875,7 +1874,7 @@
       <c r="A8" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>0.1388888888888889</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1887,7 +1886,7 @@
       <c r="I8" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="23">
         <v>0.15277777777777779</v>
       </c>
       <c r="K8" t="s">
@@ -1898,7 +1897,7 @@
       <c r="A9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>0.1388888888888889</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1910,7 +1909,7 @@
       <c r="I9" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="23">
         <v>0.15277777777777779</v>
       </c>
       <c r="K9" t="s">
@@ -1921,7 +1920,7 @@
       <c r="A10" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>0.1388888888888889</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -1933,7 +1932,7 @@
       <c r="I10" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J10" s="23">
         <v>0.15277777777777779</v>
       </c>
       <c r="K10" t="s">
@@ -1944,7 +1943,7 @@
       <c r="A11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <v>0.1388888888888889</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -1956,7 +1955,7 @@
       <c r="I11" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="J11" s="24">
+      <c r="J11" s="23">
         <v>0.15277777777777779</v>
       </c>
       <c r="K11" t="s">
@@ -1967,7 +1966,7 @@
       <c r="A12" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>0.1388888888888889</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -1979,7 +1978,7 @@
       <c r="I12" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="J12" s="24">
+      <c r="J12" s="23">
         <v>0.15277777777777779</v>
       </c>
       <c r="K12" t="s">
@@ -1990,7 +1989,7 @@
       <c r="A13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="23">
         <v>0.1423611111111111</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -2002,7 +2001,7 @@
       <c r="I13" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="23">
         <v>0.15277777777777779</v>
       </c>
       <c r="K13" t="s">
@@ -2013,7 +2012,7 @@
       <c r="A14" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <v>0.1423611111111111</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -2025,7 +2024,7 @@
       <c r="I14" t="s">
         <v>63</v>
       </c>
-      <c r="J14" s="24">
+      <c r="J14" s="23">
         <v>0.15625</v>
       </c>
       <c r="K14" t="s">
@@ -2036,7 +2035,7 @@
       <c r="A15" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <v>0.1423611111111111</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -2050,7 +2049,7 @@
       <c r="A16" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>0.1423611111111111</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -2064,7 +2063,7 @@
       <c r="A17" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <v>0.1423611111111111</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -2078,7 +2077,7 @@
       <c r="A18" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="23">
         <v>0.1423611111111111</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -2133,7 +2132,7 @@
       <c r="A2" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>0.15972222222222221</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -2164,14 +2163,14 @@
       <c r="A3" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>0.15972222222222221</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>188</v>
       </c>
       <c r="D3" s="16"/>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="22" t="s">
         <v>79</v>
       </c>
       <c r="F3" s="10">
@@ -2186,7 +2185,7 @@
       <c r="A4" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>0.15972222222222221</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -2210,7 +2209,7 @@
       <c r="A5" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>0.15972222222222221</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -2234,7 +2233,7 @@
       <c r="A6" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>0.15972222222222221</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -2244,7 +2243,7 @@
       <c r="E6" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="23">
         <v>0.1701388888888889</v>
       </c>
       <c r="G6" s="10" t="s">
@@ -2258,7 +2257,7 @@
       <c r="A7" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>0.15972222222222221</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -2268,7 +2267,7 @@
       <c r="E7" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="23">
         <v>0.1701388888888889</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -2282,7 +2281,7 @@
       <c r="A8" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>0.16319444444444445</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -2292,7 +2291,7 @@
       <c r="E8" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="23">
         <v>0.1701388888888889</v>
       </c>
       <c r="G8" s="10" t="s">
@@ -2306,7 +2305,7 @@
       <c r="A9" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>0.16319444444444445</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -2322,7 +2321,7 @@
       <c r="A10" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>0.16319444444444445</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -2338,7 +2337,7 @@
       <c r="A11" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <v>0.16319444444444445</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -2354,7 +2353,7 @@
       <c r="A12" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>0.16319444444444445</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -2370,7 +2369,7 @@
       <c r="A13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="23">
         <v>0.16319444444444445</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -2386,7 +2385,7 @@
       <c r="A14" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <v>0.16319444444444445</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -2402,7 +2401,7 @@
       <c r="A15" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <v>0.16666666666666666</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -2416,7 +2415,7 @@
       <c r="A16" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>0.16666666666666666</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -2430,7 +2429,7 @@
       <c r="A17" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <v>0.16666666666666666</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -2444,7 +2443,7 @@
       <c r="A18" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="23">
         <v>0.16666666666666666</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -2458,7 +2457,7 @@
       <c r="A19" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="23">
         <v>0.16666666666666666</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -2471,7 +2470,7 @@
       <c r="A20" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="24">
+      <c r="B20" s="23">
         <v>0.16666666666666666</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -2488,7 +2487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8352AF9-9612-0B4B-8ABC-2826DBFDC399}">
   <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -2538,7 +2537,7 @@
       <c r="A2" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>0.17708333333333334</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -2548,7 +2547,7 @@
       <c r="E2" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="23">
         <v>0.18402777777777779</v>
       </c>
       <c r="G2" s="10" t="s">
@@ -2558,7 +2557,7 @@
       <c r="I2" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="23">
         <v>0.1875</v>
       </c>
       <c r="K2" s="10" t="s">
@@ -2568,7 +2567,7 @@
       <c r="M2" t="s">
         <v>111</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O2" s="10" t="s">
@@ -2578,7 +2577,7 @@
       <c r="Q2" t="s">
         <v>124</v>
       </c>
-      <c r="R2" s="24">
+      <c r="R2" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="S2" t="s">
@@ -2589,7 +2588,7 @@
       <c r="A3" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>0.17708333333333334</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -2599,7 +2598,7 @@
       <c r="E3" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="23">
         <v>0.18402777777777779</v>
       </c>
       <c r="G3" s="10" t="s">
@@ -2609,7 +2608,7 @@
       <c r="I3" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="23">
         <v>0.1875</v>
       </c>
       <c r="K3" s="10" t="s">
@@ -2619,7 +2618,7 @@
       <c r="M3" t="s">
         <v>112</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O3" s="10" t="s">
@@ -2629,7 +2628,7 @@
       <c r="Q3" t="s">
         <v>125</v>
       </c>
-      <c r="R3" s="24">
+      <c r="R3" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="S3" t="s">
@@ -2640,7 +2639,7 @@
       <c r="A4" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>0.17708333333333334</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -2650,7 +2649,7 @@
       <c r="E4" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>0.18402777777777779</v>
       </c>
       <c r="G4" s="10" t="s">
@@ -2660,7 +2659,7 @@
       <c r="I4" t="s">
         <v>54</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="23">
         <v>0.1875</v>
       </c>
       <c r="K4" s="10" t="s">
@@ -2670,7 +2669,7 @@
       <c r="M4" t="s">
         <v>113</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O4" s="10" t="s">
@@ -2680,7 +2679,7 @@
       <c r="Q4" t="s">
         <v>126</v>
       </c>
-      <c r="R4" s="24">
+      <c r="R4" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="S4" t="s">
@@ -2691,7 +2690,7 @@
       <c r="A5" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>0.17708333333333334</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -2701,7 +2700,7 @@
       <c r="E5" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>0.18402777777777779</v>
       </c>
       <c r="G5" s="10" t="s">
@@ -2711,7 +2710,7 @@
       <c r="I5" t="s">
         <v>55</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="23">
         <v>0.1875</v>
       </c>
       <c r="K5" s="10" t="s">
@@ -2721,7 +2720,7 @@
       <c r="M5" t="s">
         <v>114</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O5" s="10" t="s">
@@ -2731,7 +2730,7 @@
       <c r="Q5" t="s">
         <v>127</v>
       </c>
-      <c r="R5" s="24">
+      <c r="R5" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="S5" t="s">
@@ -2742,7 +2741,7 @@
       <c r="A6" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>0.17708333333333334</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -2752,7 +2751,7 @@
       <c r="E6" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="23">
         <v>0.18402777777777779</v>
       </c>
       <c r="G6" s="10" t="s">
@@ -2762,7 +2761,7 @@
       <c r="I6" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="23">
         <v>0.1875</v>
       </c>
       <c r="K6" s="10" t="s">
@@ -2772,7 +2771,7 @@
       <c r="M6" t="s">
         <v>115</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O6" s="10" t="s">
@@ -2782,7 +2781,7 @@
       <c r="Q6" t="s">
         <v>128</v>
       </c>
-      <c r="R6" s="24">
+      <c r="R6" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="S6" t="s">
@@ -2793,7 +2792,7 @@
       <c r="A7" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>0.17708333333333334</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -2803,7 +2802,7 @@
       <c r="E7" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="23">
         <v>0.18402777777777779</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -2817,7 +2816,7 @@
       <c r="M7" t="s">
         <v>116</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O7" s="10" t="s">
@@ -2827,7 +2826,7 @@
       <c r="Q7" t="s">
         <v>129</v>
       </c>
-      <c r="R7" s="24">
+      <c r="R7" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="S7" t="s">
@@ -2838,7 +2837,7 @@
       <c r="A8" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>0.17708333333333334</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -2848,7 +2847,7 @@
       <c r="E8" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="23">
         <v>0.18402777777777779</v>
       </c>
       <c r="G8" s="10" t="s">
@@ -2862,7 +2861,7 @@
       <c r="M8" t="s">
         <v>117</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O8" s="10" t="s">
@@ -2872,7 +2871,7 @@
       <c r="Q8" t="s">
         <v>130</v>
       </c>
-      <c r="R8" s="24">
+      <c r="R8" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="S8" t="s">
@@ -2883,7 +2882,7 @@
       <c r="A9" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>0.17708333333333334</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -2893,7 +2892,7 @@
       <c r="E9" t="s">
         <v>109</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="23">
         <v>0.18402777777777779</v>
       </c>
       <c r="G9" s="10" t="s">
@@ -2907,7 +2906,7 @@
       <c r="M9" t="s">
         <v>118</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O9" s="10" t="s">
@@ -2917,7 +2916,7 @@
       <c r="Q9" t="s">
         <v>131</v>
       </c>
-      <c r="R9" s="24">
+      <c r="R9" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="S9" t="s">
@@ -2928,7 +2927,7 @@
       <c r="A10" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>0.17708333333333334</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -2944,7 +2943,7 @@
       <c r="M10" t="s">
         <v>119</v>
       </c>
-      <c r="N10" s="24">
+      <c r="N10" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O10" s="10" t="s">
@@ -2957,7 +2956,7 @@
       <c r="A11" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <v>0.17708333333333334</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -2973,7 +2972,7 @@
       <c r="M11" t="s">
         <v>120</v>
       </c>
-      <c r="N11" s="24">
+      <c r="N11" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O11" s="10" t="s">
@@ -2986,7 +2985,7 @@
       <c r="A12" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>0.18055555555555555</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -3002,7 +3001,7 @@
       <c r="M12" t="s">
         <v>121</v>
       </c>
-      <c r="N12" s="24">
+      <c r="N12" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O12" s="10" t="s">
@@ -3015,7 +3014,7 @@
       <c r="A13" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="23">
         <v>0.18055555555555555</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -3031,7 +3030,7 @@
       <c r="M13" t="s">
         <v>122</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O13" s="10" t="s">
@@ -3044,7 +3043,7 @@
       <c r="A14" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <v>0.18055555555555555</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -3060,7 +3059,7 @@
       <c r="M14" t="s">
         <v>123</v>
       </c>
-      <c r="N14" s="24">
+      <c r="N14" s="23">
         <v>0.19097222222222221</v>
       </c>
       <c r="O14" s="10" t="s">
@@ -3073,7 +3072,7 @@
       <c r="A15" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <v>0.18055555555555555</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -3091,7 +3090,7 @@
       <c r="A16" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>0.18055555555555555</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -3109,7 +3108,7 @@
       <c r="A17" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <v>0.18055555555555555</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -3127,7 +3126,7 @@
       <c r="A18" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="23">
         <v>0.18055555555555555</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -3145,7 +3144,7 @@
       <c r="A19" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="23">
         <v>0.18055555555555555</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -3162,7 +3161,7 @@
       <c r="A20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="24">
+      <c r="B20" s="23">
         <v>0.18055555555555555</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -3179,7 +3178,7 @@
       <c r="A21" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21" s="23">
         <v>0.18055555555555555</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -3196,7 +3195,7 @@
       <c r="A22" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="24">
+      <c r="B22" s="23">
         <v>0.18055555555555555</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -3209,7 +3208,7 @@
       <c r="P22" s="16"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="24" t="s">
         <v>73</v>
       </c>
       <c r="B23" s="20">
@@ -3279,7 +3278,7 @@
       <c r="A2" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="C2" t="s">
@@ -3294,7 +3293,7 @@
       <c r="A3" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="C3" t="s">
@@ -3306,7 +3305,7 @@
       <c r="A4" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="C4" t="s">
@@ -3318,7 +3317,7 @@
       <c r="A5" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="C5" t="s">
@@ -3330,7 +3329,7 @@
       <c r="A6" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>0.19444444444444445</v>
       </c>
       <c r="C6" t="s">
@@ -3440,10 +3439,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C2FEDC-8C44-A345-8039-FB37E4511882}">
-  <dimension ref="A1:N1048576"/>
+  <dimension ref="A1:N1048575"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3467,7 +3466,7 @@
       <c r="A2" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>0.20833333333333334</v>
       </c>
       <c r="C2" t="s">
@@ -3479,7 +3478,7 @@
       <c r="A3" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>0.20972222222222223</v>
       </c>
       <c r="C3" t="s">
@@ -3491,7 +3490,7 @@
       <c r="A4" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>0.21180555555555555</v>
       </c>
       <c r="C4" t="s">
@@ -3501,9 +3500,9 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="B5" s="24">
+        <v>197</v>
+      </c>
+      <c r="B5" s="23">
         <v>0.21527777777777779</v>
       </c>
       <c r="C5" t="s">
@@ -3513,19 +3512,26 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="23">
+        <v>0.21875</v>
+      </c>
+      <c r="C6" t="s">
+        <v>169</v>
+      </c>
+      <c r="N6" s="10"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="B6" s="24">
-        <v>0.21527777777777779</v>
-      </c>
-      <c r="C6" t="s">
-        <v>175</v>
-      </c>
-      <c r="N6" s="10"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="10"/>
+      <c r="B7" s="23">
+        <v>0.21875</v>
+      </c>
+      <c r="C7" t="s">
+        <v>169</v>
+      </c>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -3536,7 +3542,6 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="15"/>
       <c r="B9" s="10"/>
-      <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="15"/>
@@ -3592,7 +3597,6 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
-      <c r="B23" s="10"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
@@ -3609,11 +3613,8 @@
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
-    </row>
-    <row r="1048576" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H1048576" s="10">
+    <row r="1048575" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H1048575" s="10">
         <v>0.1875</v>
       </c>
     </row>
@@ -3648,7 +3649,7 @@
       <c r="A2" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>0.21875</v>
       </c>
       <c r="C2" t="s">
@@ -3659,7 +3660,7 @@
       <c r="A3" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>0.21875</v>
       </c>
       <c r="C3" t="s">
@@ -3670,7 +3671,7 @@
       <c r="A4" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>0.21875</v>
       </c>
       <c r="C4" t="s">
@@ -3681,7 +3682,7 @@
       <c r="A5" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>0.21875</v>
       </c>
       <c r="C5" t="s">
@@ -3692,7 +3693,7 @@
       <c r="A6" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>0.21875</v>
       </c>
       <c r="C6" t="s">
@@ -3703,7 +3704,7 @@
       <c r="A7" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>0.21875</v>
       </c>
       <c r="C7" t="s">
@@ -3714,7 +3715,7 @@
       <c r="A8" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>0.22222222222222221</v>
       </c>
       <c r="C8" t="s">
@@ -3725,7 +3726,7 @@
       <c r="A9" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>0.22222222222222221</v>
       </c>
       <c r="C9" t="s">
@@ -3736,7 +3737,7 @@
       <c r="A10" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>0.22222222222222221</v>
       </c>
       <c r="C10" t="s">
@@ -3747,7 +3748,7 @@
       <c r="A11" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <v>0.22222222222222221</v>
       </c>
       <c r="C11" t="s">
@@ -3758,7 +3759,7 @@
       <c r="A12" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>0.22222222222222221</v>
       </c>
       <c r="C12" t="s">
@@ -3769,7 +3770,7 @@
       <c r="A13" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="23">
         <v>0.22916666666666666</v>
       </c>
       <c r="C13" t="s">
@@ -3780,7 +3781,7 @@
       <c r="A14" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <v>0.22916666666666666</v>
       </c>
       <c r="C14" t="s">
@@ -3791,7 +3792,7 @@
       <c r="A15" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <v>0.22916666666666666</v>
       </c>
       <c r="C15" t="s">
@@ -3802,7 +3803,7 @@
       <c r="A16" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>0.22916666666666666</v>
       </c>
       <c r="C16" t="s">
@@ -3813,7 +3814,7 @@
       <c r="A17" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <v>0.22916666666666666</v>
       </c>
       <c r="C17" t="s">
@@ -3824,7 +3825,7 @@
       <c r="A18" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="23">
         <v>0.22916666666666666</v>
       </c>
       <c r="C18" t="s">
@@ -3909,7 +3910,7 @@
       <c r="A2" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>0.23958333333333334</v>
       </c>
       <c r="C2" t="s">
@@ -3920,7 +3921,7 @@
       <c r="A3" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>0.24305555555555555</v>
       </c>
       <c r="C3" t="s">
@@ -3931,7 +3932,7 @@
       <c r="A4" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>0.25</v>
       </c>
       <c r="C4" t="s">
@@ -4078,7 +4079,7 @@
       <c r="A2" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>0.26041666666666669</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -4088,7 +4089,7 @@
       <c r="E2" t="s">
         <v>160</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="23">
         <v>0.2673611111111111</v>
       </c>
       <c r="G2" t="s">
@@ -4100,7 +4101,7 @@
       <c r="A3" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>0.26041666666666669</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -4110,7 +4111,7 @@
       <c r="E3" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="23">
         <v>0.27083333333333331</v>
       </c>
       <c r="G3" t="s">
@@ -4122,7 +4123,7 @@
       <c r="A4" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>0.26041666666666669</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -4132,7 +4133,7 @@
       <c r="E4" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>0.27083333333333331</v>
       </c>
       <c r="G4" t="s">
@@ -4144,7 +4145,7 @@
       <c r="A5" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>0.26041666666666669</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -4154,7 +4155,7 @@
       <c r="E5" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>0.27083333333333331</v>
       </c>
       <c r="G5" t="s">
@@ -4166,7 +4167,7 @@
       <c r="A6" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>0.26041666666666669</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -4176,7 +4177,7 @@
       <c r="E6" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="23">
         <v>0.27083333333333331</v>
       </c>
       <c r="G6" t="s">
@@ -4188,7 +4189,7 @@
       <c r="A7" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>0.26041666666666669</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -4198,7 +4199,7 @@
       <c r="E7" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="23">
         <v>0.27083333333333331</v>
       </c>
       <c r="G7" t="s">
@@ -4210,7 +4211,7 @@
       <c r="A8" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>0.26041666666666669</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -4220,7 +4221,7 @@
       <c r="E8" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="23">
         <v>0.27083333333333331</v>
       </c>
       <c r="G8" t="s">
@@ -4232,7 +4233,7 @@
       <c r="A9" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>0.26041666666666669</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -4242,7 +4243,7 @@
       <c r="E9" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="23">
         <v>0.27430555555555558</v>
       </c>
       <c r="G9" t="s">
@@ -4254,7 +4255,7 @@
       <c r="A10" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>0.2638888888888889</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -4267,7 +4268,7 @@
       <c r="A11" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <v>0.2638888888888889</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -4280,7 +4281,7 @@
       <c r="A12" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>0.2638888888888889</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -4293,7 +4294,7 @@
       <c r="A13" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="23">
         <v>0.2638888888888889</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -4306,7 +4307,7 @@
       <c r="A14" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <v>0.2638888888888889</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -4319,7 +4320,7 @@
       <c r="A15" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <v>0.2638888888888889</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -4332,7 +4333,7 @@
       <c r="A16" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>0.2638888888888889</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -4345,7 +4346,7 @@
       <c r="A17" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <v>0.2638888888888889</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -4358,7 +4359,7 @@
       <c r="A18" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="23">
         <v>0.2638888888888889</v>
       </c>
       <c r="C18" s="10" t="s">

</xml_diff>

<commit_message>
remioved excel temp file
</commit_message>
<xml_diff>
--- a/SSPHP Documentation/20241203_DCAP_Scheduling.xlsx
+++ b/SSPHP Documentation/20241203_DCAP_Scheduling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianpearl/GITHUB/service-security-posture-hardening/SSPHP Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A33BA4-02D7-E04B-AA9A-CFD41D8AE14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71B686E-4998-A148-B9FF-5F8D91BC30E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="5" xr2:uid="{E019FE81-96E6-EA40-88B3-D10E9033B9A2}"/>
+    <workbookView xWindow="17720" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="9" xr2:uid="{E019FE81-96E6-EA40-88B3-D10E9033B9A2}"/>
   </bookViews>
   <sheets>
     <sheet name="OVERALL" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="200">
   <si>
     <t>Starts</t>
   </si>
@@ -650,6 +650,12 @@
   </si>
   <si>
     <t>ssphp_create_bdmc_csv_DEV</t>
+  </si>
+  <si>
+    <t>0 * * * *</t>
+  </si>
+  <si>
+    <t>every hour</t>
   </si>
 </sst>
 </file>
@@ -1466,8 +1472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB4B2C4-9630-254C-A643-5533F7B8AEF0}">
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1506,11 +1512,11 @@
       <c r="A3" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="23">
-        <v>0.29166666666666669</v>
+      <c r="B3" s="23" t="s">
+        <v>199</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="M3" s="15"/>
       <c r="N3" s="10"/>
@@ -3441,8 +3447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C2FEDC-8C44-A345-8039-FB37E4511882}">
   <dimension ref="A1:N1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>